<commit_message>
generacion de documentos Word con datos del excel (por ahora solo funcion con un word en la misma carpeta y con el nombre plantilla)
</commit_message>
<xml_diff>
--- a/app/clientes.xlsx
+++ b/app/clientes.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oo199\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B25188-9115-4A00-8B87-6A00AA3BE849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="CLIENTES" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="CLIENTES"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>NOMBRE_EMPRESA</t>
   </si>
@@ -49,7 +43,7 @@
     <t>REPRESENTANTE_LEGAL</t>
   </si>
   <si>
-    <t>REP_LEGAL_IDENTIFICACION</t>
+    <t>CEDULA_REPR</t>
   </si>
   <si>
     <t>REP_LEGAL_DIRECCION</t>
@@ -98,21 +92,6 @@
   </si>
   <si>
     <t>TELEFONO_BANCO</t>
-  </si>
-  <si>
-    <t>GRAN_CONTRIBUYENTE</t>
-  </si>
-  <si>
-    <t>RET_IVA</t>
-  </si>
-  <si>
-    <t>RET_ICA</t>
-  </si>
-  <si>
-    <t>RET_RENTA</t>
-  </si>
-  <si>
-    <t>FECHA_DILIGENCIAMIENTO</t>
   </si>
   <si>
     <t>NOMBRE_FIRMANTE</t>
@@ -198,22 +177,14 @@
   </si>
   <si>
     <t>018000912345</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Sí</t>
-  </si>
-  <si>
-    <t>2025-01-10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,10 +195,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -238,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -248,54 +230,82 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+  <cellXfs count="10">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -328,79 +338,79 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -421,54 +431,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -478,7 +487,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -487,7 +496,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -496,7 +505,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -504,10 +513,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -536,7 +545,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -549,13 +558,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -573,16 +581,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +655,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -667,118 +706,89 @@
       <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33.75">
+      <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G2" t="s">
+      <c r="L2" s="4">
+        <v>4783</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H2" t="s">
+      <c r="N2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I2" t="s">
+      <c r="O2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J2" t="s">
+      <c r="P2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K2" t="s">
+      <c r="Q2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L2">
-        <v>4783</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="R2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N2" t="s">
+      <c r="S2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="O2" t="s">
+      <c r="T2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="P2" t="s">
+      <c r="U2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="V2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="R2" t="s">
+      <c r="W2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="S2" t="s">
+      <c r="X2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="T2" t="s">
+      <c r="Y2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="U2" t="s">
+      <c r="Z2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="V2" t="s">
-        <v>52</v>
-      </c>
-      <c r="W2" t="s">
-        <v>53</v>
-      </c>
-      <c r="X2" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>41</v>
+      <c r="AA2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mejora visual y funcionalidad de genracion correctamente implentada
</commit_message>
<xml_diff>
--- a/app/clientes.xlsx
+++ b/app/clientes.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oo199\Desktop\Genera Documentos\app\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED25DA6-14D3-4A77-A322-6B7FDEA2A009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="CLIENTES"/>
+    <sheet name="CLIENTES" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>NOMBRE_EMPRESA</t>
   </si>
@@ -101,13 +107,120 @@
   </si>
   <si>
     <t>10203040</t>
+  </si>
+  <si>
+    <t>Agroindustrial del Valle S.A.</t>
+  </si>
+  <si>
+    <t>80098765-4</t>
+  </si>
+  <si>
+    <t>RUT-2023-002</t>
+  </si>
+  <si>
+    <t>Carrera 7 #12-45</t>
+  </si>
+  <si>
+    <t>Cali</t>
+  </si>
+  <si>
+    <t>info@agrovalle.com</t>
+  </si>
+  <si>
+    <t>María López Ruiz</t>
+  </si>
+  <si>
+    <t>Av. 4N #10-30 Cali</t>
+  </si>
+  <si>
+    <t>Banco de Bogotá</t>
+  </si>
+  <si>
+    <t>Tecnología Global Ltda.</t>
+  </si>
+  <si>
+    <t>90123456-7</t>
+  </si>
+  <si>
+    <t>RUT-2023-003</t>
+  </si>
+  <si>
+    <t>Av. El Dorado #68-10</t>
+  </si>
+  <si>
+    <t>soporte@tecnoglobal.co</t>
+  </si>
+  <si>
+    <t>Carlos Sánchez Mendoza</t>
+  </si>
+  <si>
+    <t>Calle 100 #15-80 Bogotá</t>
+  </si>
+  <si>
+    <t>Davivienda</t>
+  </si>
+  <si>
+    <t>Carlos Sánchez</t>
+  </si>
+  <si>
+    <t>Logística Express S.A.S</t>
+  </si>
+  <si>
+    <t>70012345-8</t>
+  </si>
+  <si>
+    <t>RUT-2023-004</t>
+  </si>
+  <si>
+    <t>Transversal 20 #30-1</t>
+  </si>
+  <si>
+    <t>Medellín</t>
+  </si>
+  <si>
+    <t>contacto@logexpress.co</t>
+  </si>
+  <si>
+    <t>Ana Gómez Torres</t>
+  </si>
+  <si>
+    <t>Cra 43A #5-120 Medellín</t>
+  </si>
+  <si>
+    <t>BBVA</t>
+  </si>
+  <si>
+    <t>Constructora Norte S.A.</t>
+  </si>
+  <si>
+    <t>60054321-9</t>
+  </si>
+  <si>
+    <t>RUT-2023-005</t>
+  </si>
+  <si>
+    <t>Calle 90 #11-15</t>
+  </si>
+  <si>
+    <t>Barranquilla</t>
+  </si>
+  <si>
+    <t>obra@constructoranorte</t>
+  </si>
+  <si>
+    <t>Ricardo Vargas Díaz</t>
+  </si>
+  <si>
+    <t>Cra 50 #80-100 Barranquilla</t>
+  </si>
+  <si>
+    <t>Scotiabank Colpatria</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -172,44 +285,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -220,10 +333,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -261,71 +374,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -353,7 +466,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -376,11 +489,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -389,13 +502,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -405,7 +518,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -414,7 +527,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -423,7 +536,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -431,10 +544,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -499,43 +612,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="35.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="24.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="25.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="2" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="17" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -547,7 +656,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -559,7 +668,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -581,55 +690,266 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33.75">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>10203040</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="7">
         <v>3001234567</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="7">
         <v>4783</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4" t="s">
+      <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="6">
+        <v>55667788</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="8">
+        <v>3105556677</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="8">
+        <v>121</v>
+      </c>
+      <c r="L3">
+        <v>50000000</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3">
+        <v>98765432109</v>
+      </c>
+      <c r="O3">
+        <v>18000112233</v>
+      </c>
+      <c r="P3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3">
+        <v>55667788</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="6">
+        <v>99887766</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="8">
+        <v>3209988776</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="8">
+        <v>6201</v>
+      </c>
+      <c r="L4">
+        <v>25000000</v>
+      </c>
+      <c r="M4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4">
+        <v>45678912345</v>
+      </c>
+      <c r="O4">
+        <v>18000987654</v>
+      </c>
+      <c r="P4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4">
+        <v>99887766</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="6">
+        <v>33445566</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="8">
+        <v>3003344556</v>
+      </c>
+      <c r="H5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="8">
+        <v>4923</v>
+      </c>
+      <c r="L5">
+        <v>15000000</v>
+      </c>
+      <c r="M5" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5">
+        <v>11223344556</v>
+      </c>
+      <c r="O5">
+        <v>18000556677</v>
+      </c>
+      <c r="P5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q5">
+        <v>33445566</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="6">
+        <v>11223344</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="8">
+        <v>3501122334</v>
+      </c>
+      <c r="H6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="8">
+        <v>4100</v>
+      </c>
+      <c r="L6">
+        <v>75000000</v>
+      </c>
+      <c r="M6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6">
+        <v>55443322110</v>
+      </c>
+      <c r="O6">
+        <v>18000334455</v>
+      </c>
+      <c r="P6" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q6">
+        <v>11223344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creacion de la vista clientes y la visualizacion de la lista y sus detalles
</commit_message>
<xml_diff>
--- a/app/clientes.xlsx
+++ b/app/clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oo199\Desktop\Genera Documentos\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED25DA6-14D3-4A77-A322-6B7FDEA2A009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AF9E5D-5B3E-4F42-BFE0-B31057AFA8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -251,7 +251,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -281,11 +281,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -293,23 +321,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,44 +644,42 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="17" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -668,7 +691,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -697,7 +720,7 @@
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="3">
         <v>10203040</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -709,7 +732,7 @@
       <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="4">
         <v>3001234567</v>
       </c>
       <c r="H2" t="s">
@@ -721,7 +744,7 @@
       <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="4">
         <v>4783</v>
       </c>
       <c r="M2" t="s">
@@ -747,7 +770,7 @@
       <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="2">
         <v>55667788</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -759,7 +782,7 @@
       <c r="F3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="5">
         <v>3105556677</v>
       </c>
       <c r="H3" t="s">
@@ -771,7 +794,7 @@
       <c r="J3" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="5">
         <v>121</v>
       </c>
       <c r="L3">
@@ -800,7 +823,7 @@
       <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="2">
         <v>99887766</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -812,7 +835,7 @@
       <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="5">
         <v>3209988776</v>
       </c>
       <c r="H4" t="s">
@@ -824,7 +847,7 @@
       <c r="J4" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="5">
         <v>6201</v>
       </c>
       <c r="L4">
@@ -853,7 +876,7 @@
       <c r="B5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="2">
         <v>33445566</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -865,7 +888,7 @@
       <c r="F5" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="5">
         <v>3003344556</v>
       </c>
       <c r="H5" t="s">
@@ -877,7 +900,7 @@
       <c r="J5" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="5">
         <v>4923</v>
       </c>
       <c r="L5">
@@ -906,7 +929,7 @@
       <c r="B6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="2">
         <v>11223344</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -918,7 +941,7 @@
       <c r="F6" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="5">
         <v>3501122334</v>
       </c>
       <c r="H6" t="s">
@@ -930,7 +953,7 @@
       <c r="J6" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="5">
         <v>4100</v>
       </c>
       <c r="L6">

</xml_diff>